<commit_message>
add validation to excel parsing
</commit_message>
<xml_diff>
--- a/data/Antminer Models[90].xlsx
+++ b/data/Antminer Models[90].xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t xml:space="preserve">Bitmain Antminer T19 Hydro (145Th)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
   <si>
     <t xml:space="preserve">Date</t>
@@ -178,9 +184,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -248,7 +255,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,6 +265,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -281,8 +292,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFBBC3C8"/>
-          <bgColor rgb="FF22252C"/>
+          <fgColor rgb="FF3D3D3D"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -316,16 +327,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.69"/>
@@ -824,6 +835,22 @@
       </c>
       <c r="C45" s="0" t="n">
         <v>0.038</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -851,18 +878,18 @@
       <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>